<commit_message>
Señal para nuevo componente
</commit_message>
<xml_diff>
--- a/pangea/catalogos_capII_15_abr_21.xlsx
+++ b/pangea/catalogos_capII_15_abr_21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox (LANCIS)\CARPETAS_TRABAJO\vhernandez\repositorios_git\cap2\pangea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF28395-0A81-4934-8388-177EAE9F6B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE65C1B-0046-4A4F-B5DC-96E88ABDE05D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D5E2090E-4DC5-412E-AC60-D93F4347DA8F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="tipos" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">catálogos!$B$1:$I$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">catálogos!$B$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="108">
   <si>
     <t xml:space="preserve">Datos generales del componente </t>
   </si>
@@ -91,9 +91,6 @@
     <t>Generación de aguas residuales por tipo</t>
   </si>
   <si>
-    <t>Longitud de obra de obras lineales</t>
-  </si>
-  <si>
     <t>Operación</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Uso de sustancias químicas peligrosas por cobertura y zonificación</t>
   </si>
   <si>
-    <t xml:space="preserve">Maquinaria por cobertura y zonificación </t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>Formulario TIPO</t>
   </si>
   <si>
-    <t>Desmonte, despalme, excavación y relleno por tipo de cobertura y zonificación</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pre-requisito </t>
   </si>
   <si>
@@ -356,6 +347,21 @@
   </si>
   <si>
     <t>pendiente cats</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Longitud de obras lineales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maquinaria por zonificación </t>
+  </si>
+  <si>
+    <t>Desmonte, despalme, excavación y relleno por tipo de zonificación</t>
+  </si>
+  <si>
+    <t>Tipos de aprovechamiento por tipo de zonificación</t>
   </si>
 </sst>
 </file>
@@ -749,11 +755,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9E8254-D393-4638-B959-62062D3B4679}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,16 +780,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -792,38 +798,38 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -832,89 +838,89 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>12</v>
@@ -925,213 +931,213 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>81</v>
+        <v>12</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>104</v>
+      <c r="A12" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="I14" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="I15" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>100</v>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>103</v>
+      <c r="A18" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" s="2">
+        <v>80</v>
+      </c>
+      <c r="G19" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H20" s="2">
         <v>1</v>
@@ -1139,385 +1145,400 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>103</v>
+      <c r="A32" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>103</v>
+      <c r="A33" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>103</v>
+      <c r="A34" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>103</v>
+      <c r="A35" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H38" s="2">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F43" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H43" s="2">
         <v>1</v>
@@ -1525,146 +1546,146 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G48" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G50" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H51" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G54" s="2">
+      <c r="H54" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>4</v>
@@ -1675,10 +1696,10 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>4</v>
@@ -1689,10 +1710,10 @@
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>4</v>
@@ -1700,27 +1721,42 @@
       <c r="G57" s="2">
         <v>1</v>
       </c>
-      <c r="H57" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I40" xr:uid="{FC8CF568-3DCD-407E-8CEE-2735EF8756EA}">
+  <autoFilter ref="B1:I41" xr:uid="{FC8CF568-3DCD-407E-8CEE-2735EF8756EA}">
     <filterColumn colId="1">
-      <filters>
-        <filter val="Catálogo"/>
-        <filter val="Catálogo de abreviaturas"/>
-        <filter val="Catálogo por fase"/>
+      <filters blank="1">
+        <filter val="Formulario-datos"/>
+        <filter val="Formulario-datos-abreviaturas"/>
+        <filter val="Formulario-texto-figuras"/>
+        <filter val="PNG"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1758,13 +1794,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -1772,10 +1808,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G2" s="5">
         <v>20</v>
@@ -1786,7 +1822,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1797,7 +1833,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1808,7 +1844,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1819,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1846,24 +1882,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1871,7 +1907,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1879,7 +1915,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1890,7 +1926,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1899,12 +1935,12 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1916,12 +1952,12 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1930,12 +1966,12 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1944,12 +1980,12 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1958,12 +1994,12 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>1</v>

</xml_diff>